<commit_message>
Working Azerty Caps and Yellow Vowels
</commit_message>
<xml_diff>
--- a/docs/CAPS/CapsLayers.xlsx
+++ b/docs/CAPS/CapsLayers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Cameroon-Keyboard\docs\CAPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{059882D4-5913-4A6E-B7F5-8DE4D8F0B567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA640FC-C2B2-4EFE-9104-33BB9CEC1BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="17070" xr2:uid="{B5C0FECB-9AE4-4306-B37E-DBCCCD134AAA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="47">
   <si>
     <t>shift-L</t>
   </si>
@@ -92,9 +92,6 @@
     <t>icon: ƏŊƆ</t>
   </si>
   <si>
-    <t>icon: ShiftLocked</t>
-  </si>
-  <si>
     <t xml:space="preserve">Special (active) </t>
   </si>
   <si>
@@ -128,9 +125,6 @@
     <t>NextLayer</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -156,13 +150,40 @@
   </si>
   <si>
     <t>Caps</t>
+  </si>
+  <si>
+    <t>* Note:  After typing symbols not associated with phone numbers, the KB returns to default.</t>
+  </si>
+  <si>
+    <t>* Note:  After typing symbols not associated with phone numbers, the KB returns to caps.</t>
+  </si>
+  <si>
+    <t>*Note, The individual letters on this layer don't have a nextlayer, only the modifiers.</t>
+  </si>
+  <si>
+    <t>* Note:  After typing each individual letter, the KB returns to default.</t>
+  </si>
+  <si>
+    <t>* Note, The individual letters on this layer don't have a nextlayer, only the modifiers.</t>
+  </si>
+  <si>
+    <t>* Note:  After typing each individual letter, the KB returns to rightalt.</t>
+  </si>
+  <si>
+    <t>* Note:  After typing each individual letter, the KB returns to caps.</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>icon: ShiftedLocked</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,8 +206,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,6 +232,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -208,16 +249,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -232,7 +277,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor rgb="FFFF7C80"/>
         </patternFill>
       </fill>
     </dxf>
@@ -551,47 +596,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99DB43F7-765C-41E7-B9CF-D83B3234F17D}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I19" sqref="I19"/>
+      <selection pane="bottomLeft" activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -599,22 +646,22 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
       <c r="G2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -622,22 +669,22 @@
         <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
       <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>3</v>
-      </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -645,22 +692,22 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -668,22 +715,22 @@
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>3</v>
-      </c>
       <c r="G5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -691,22 +738,22 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>3</v>
-      </c>
       <c r="G6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -714,137 +761,119 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
       </c>
       <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
         <v>12</v>
       </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" t="s">
-        <v>3</v>
-      </c>
       <c r="G7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" t="s">
-        <v>31</v>
+      <c r="A8" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>37</v>
+      <c r="B9" t="s">
+        <v>34</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
-      <c r="B10" t="s">
-        <v>36</v>
+      <c r="B10" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="G10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>37</v>
+      <c r="B11" t="s">
+        <v>34</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F11" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="G11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" t="s">
-        <v>36</v>
+      <c r="B12" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="F12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -852,68 +881,50 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F13" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" t="s">
-        <v>31</v>
+      <c r="A15" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -921,22 +932,22 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F16" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="G16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -944,143 +955,122 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F17" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="G17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>37</v>
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" t="s">
         <v>20</v>
       </c>
-      <c r="E19" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" t="s">
-        <v>3</v>
-      </c>
       <c r="G19" t="s">
-        <v>33</v>
-      </c>
-      <c r="H19" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F20" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" t="s">
-        <v>31</v>
+      <c r="A20" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>37</v>
+      <c r="B21" t="s">
+        <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F21" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="G21" t="s">
-        <v>33</v>
-      </c>
-      <c r="H21" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
-      <c r="B22" t="s">
-        <v>36</v>
+      <c r="B22" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E22" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F22" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G22" t="s">
         <v>31</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1088,308 +1078,410 @@
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F23" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="G23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>36</v>
+        <v>9</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E24" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="F24" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G24" t="s">
         <v>31</v>
       </c>
+      <c r="H24" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" t="s">
-        <v>0</v>
-      </c>
-      <c r="D25" t="s">
-        <v>20</v>
-      </c>
       <c r="E25" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F25" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="G25" t="s">
-        <v>33</v>
-      </c>
-      <c r="H25" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D26" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E26" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="F26" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G26" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" t="s">
-        <v>5</v>
-      </c>
-      <c r="F27" t="s">
-        <v>3</v>
-      </c>
-      <c r="G27" t="s">
-        <v>33</v>
-      </c>
-      <c r="H27" t="s">
-        <v>39</v>
+      <c r="A27" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E28" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F28" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="G28" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" t="s">
-        <v>36</v>
+        <v>21</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="C29" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E29" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F29" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="G29" t="s">
         <v>31</v>
       </c>
+      <c r="H29" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" t="s">
         <v>9</v>
       </c>
-      <c r="E30" t="s">
-        <v>18</v>
-      </c>
-      <c r="F30" t="s">
-        <v>16</v>
-      </c>
       <c r="G30" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B31" t="s">
-        <v>36</v>
+        <v>21</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E31" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F31" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G31" t="s">
         <v>31</v>
       </c>
+      <c r="H31" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C32" t="s">
         <v>8</v>
       </c>
       <c r="D32" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" t="s">
         <v>1</v>
       </c>
-      <c r="E32" t="s">
-        <v>24</v>
-      </c>
-      <c r="F32" t="s">
-        <v>16</v>
-      </c>
       <c r="G32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C33" t="s">
         <v>11</v>
       </c>
       <c r="D33" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E33" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F33" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="G33" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>12</v>
-      </c>
-      <c r="B34" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34" t="s">
-        <v>14</v>
-      </c>
-      <c r="E34" t="s">
-        <v>23</v>
-      </c>
-      <c r="F34" t="s">
-        <v>19</v>
-      </c>
-      <c r="G34" t="s">
-        <v>31</v>
+      <c r="A34" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" t="s">
+        <v>46</v>
+      </c>
+      <c r="E35" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" t="s">
+        <v>46</v>
+      </c>
+      <c r="E36" t="s">
+        <v>16</v>
+      </c>
+      <c r="F36" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" t="s">
+        <v>23</v>
+      </c>
+      <c r="E37" t="s">
+        <v>16</v>
+      </c>
+      <c r="F37" t="s">
+        <v>1</v>
+      </c>
+      <c r="G37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" t="s">
+        <v>3</v>
+      </c>
+      <c r="F38" t="s">
+        <v>20</v>
+      </c>
+      <c r="G38" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>12</v>
       </c>
-      <c r="B35" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="B40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40" t="s">
         <v>8</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D40" t="s">
+        <v>22</v>
+      </c>
+      <c r="E40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" t="s">
+        <v>14</v>
+      </c>
+      <c r="G40" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" t="s">
+        <v>23</v>
+      </c>
+      <c r="E42" t="s">
+        <v>16</v>
+      </c>
+      <c r="F42" t="s">
         <v>4</v>
       </c>
-      <c r="E35" t="s">
-        <v>24</v>
-      </c>
-      <c r="F35" t="s">
-        <v>16</v>
-      </c>
-      <c r="G35" t="s">
-        <v>34</v>
+      <c r="G42" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1 A2:G35 H19 H21 H27 H25 H32:H33">
+  <conditionalFormatting sqref="B1 H22 H24 H31 H29 H37:H38 A2:G42">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"N"</formula>
     </cfRule>

</xml_diff>